<commit_message>
Update fix bug qmm016
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -44620,8 +44620,8 @@
   </sheetPr>
   <dimension ref="B1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="25" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="M26" sqref="M24:M26"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="10" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="I29" sqref="I28:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
@@ -44639,8 +44639,8 @@
     <col min="15" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="12.75" thickBot="1"/>
-    <row r="2" spans="2:13" ht="13.15" customHeight="1" thickTop="1">
+    <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1">
       <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
@@ -44670,7 +44670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="13.15" customHeight="1">
+    <row r="3" spans="2:13" ht="12.2" customHeight="1">
       <c r="B3" s="39"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -44684,7 +44684,7 @@
       <c r="L3" s="41"/>
       <c r="M3" s="45"/>
     </row>
-    <row r="4" spans="2:13" ht="13.15" customHeight="1">
+    <row r="4" spans="2:13" ht="12.2" customHeight="1">
       <c r="B4" s="12"/>
       <c r="C4" s="6"/>
       <c r="D4" s="22"/>
@@ -44698,7 +44698,7 @@
       <c r="L4" s="21"/>
       <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="2:13" ht="13.15" customHeight="1">
+    <row r="5" spans="2:13" ht="12.2" customHeight="1">
       <c r="B5" s="13"/>
       <c r="C5" s="5"/>
       <c r="D5" s="23"/>
@@ -44712,7 +44712,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="2:13" ht="13.15" customHeight="1">
+    <row r="6" spans="2:13" ht="12.2" customHeight="1">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="22"/>
@@ -44726,7 +44726,7 @@
       <c r="L6" s="21"/>
       <c r="M6" s="16"/>
     </row>
-    <row r="7" spans="2:13" ht="13.15" customHeight="1">
+    <row r="7" spans="2:13" ht="12.2" customHeight="1">
       <c r="B7" s="13"/>
       <c r="C7" s="5"/>
       <c r="D7" s="23"/>
@@ -44740,7 +44740,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="2:13" ht="13.15" customHeight="1">
+    <row r="8" spans="2:13" ht="12.2" customHeight="1">
       <c r="B8" s="12"/>
       <c r="C8" s="2"/>
       <c r="D8" s="22"/>
@@ -44754,7 +44754,7 @@
       <c r="L8" s="21"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="2:13" ht="13.15" customHeight="1">
+    <row r="9" spans="2:13" ht="12.2" customHeight="1">
       <c r="B9" s="13"/>
       <c r="C9" s="5"/>
       <c r="D9" s="23"/>
@@ -44768,7 +44768,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="2:13" ht="13.15" customHeight="1">
+    <row r="10" spans="2:13" ht="12.2" customHeight="1">
       <c r="B10" s="12"/>
       <c r="C10" s="2"/>
       <c r="D10" s="22"/>
@@ -44782,7 +44782,7 @@
       <c r="L10" s="21"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="2:13" ht="13.15" customHeight="1">
+    <row r="11" spans="2:13" ht="12.2" customHeight="1">
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="23"/>
@@ -44796,7 +44796,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="2:13" ht="13.15" customHeight="1">
+    <row r="12" spans="2:13" ht="12.2" customHeight="1">
       <c r="B12" s="12"/>
       <c r="C12" s="2"/>
       <c r="D12" s="22"/>
@@ -44810,7 +44810,7 @@
       <c r="L12" s="21"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="2:13" ht="13.15" customHeight="1">
+    <row r="13" spans="2:13" ht="12.2" customHeight="1">
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="23"/>
@@ -44824,7 +44824,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="2:13" ht="13.15" customHeight="1">
+    <row r="14" spans="2:13" ht="12.2" customHeight="1">
       <c r="B14" s="12"/>
       <c r="C14" s="2"/>
       <c r="D14" s="22"/>
@@ -44838,7 +44838,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="16"/>
     </row>
-    <row r="15" spans="2:13" ht="13.15" customHeight="1">
+    <row r="15" spans="2:13" ht="12.2" customHeight="1">
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="23"/>
@@ -44852,7 +44852,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="2:13" ht="13.15" customHeight="1">
+    <row r="16" spans="2:13" ht="12.2" customHeight="1">
       <c r="B16" s="12"/>
       <c r="C16" s="7"/>
       <c r="D16" s="21"/>
@@ -44866,7 +44866,7 @@
       <c r="L16" s="21"/>
       <c r="M16" s="16"/>
     </row>
-    <row r="17" spans="2:13" ht="13.15" customHeight="1">
+    <row r="17" spans="2:13" ht="12.2" customHeight="1">
       <c r="B17" s="13"/>
       <c r="C17" s="9"/>
       <c r="D17" s="23"/>
@@ -44880,7 +44880,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="2:13" ht="13.15" customHeight="1">
+    <row r="18" spans="2:13" ht="12.2" customHeight="1">
       <c r="B18" s="12"/>
       <c r="C18" s="2"/>
       <c r="D18" s="21"/>
@@ -44894,7 +44894,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="13.15" customHeight="1">
+    <row r="19" spans="2:13" ht="12.2" customHeight="1">
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="23"/>
@@ -44908,7 +44908,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="2:13" ht="13.15" customHeight="1">
+    <row r="20" spans="2:13" ht="12.2" customHeight="1">
       <c r="B20" s="12"/>
       <c r="C20" s="2"/>
       <c r="D20" s="22"/>
@@ -44922,7 +44922,7 @@
       <c r="L20" s="21"/>
       <c r="M20" s="16"/>
     </row>
-    <row r="21" spans="2:13" ht="13.15" customHeight="1">
+    <row r="21" spans="2:13" ht="12.2" customHeight="1">
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="23"/>
@@ -44936,7 +44936,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="2:13" ht="13.15" customHeight="1">
+    <row r="22" spans="2:13" ht="12.2" customHeight="1">
       <c r="B22" s="12"/>
       <c r="C22" s="2"/>
       <c r="D22" s="22"/>
@@ -44950,7 +44950,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="16"/>
     </row>
-    <row r="23" spans="2:13" ht="13.15" customHeight="1">
+    <row r="23" spans="2:13" ht="12.2" customHeight="1">
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="23"/>
@@ -44964,7 +44964,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="2:13" ht="13.15" customHeight="1">
+    <row r="24" spans="2:13" ht="12.2" customHeight="1">
       <c r="B24" s="12"/>
       <c r="C24" s="2"/>
       <c r="D24" s="22"/>
@@ -44978,7 +44978,7 @@
       <c r="L24" s="21"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="2:13" ht="13.15" customHeight="1">
+    <row r="25" spans="2:13" ht="12.2" customHeight="1">
       <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="23"/>
@@ -44992,7 +44992,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="2:13" ht="13.15" customHeight="1">
+    <row r="26" spans="2:13" ht="12.2" customHeight="1">
       <c r="B26" s="12"/>
       <c r="C26" s="2"/>
       <c r="D26" s="22"/>
@@ -45006,7 +45006,7 @@
       <c r="L26" s="21"/>
       <c r="M26" s="16"/>
     </row>
-    <row r="27" spans="2:13" ht="13.15" customHeight="1">
+    <row r="27" spans="2:13" ht="12.2" customHeight="1">
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="23"/>
@@ -45020,7 +45020,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="2:13" ht="13.15" customHeight="1">
+    <row r="28" spans="2:13" ht="12.2" customHeight="1">
       <c r="B28" s="12"/>
       <c r="C28" s="2"/>
       <c r="D28" s="22"/>
@@ -45034,7 +45034,7 @@
       <c r="L28" s="21"/>
       <c r="M28" s="16"/>
     </row>
-    <row r="29" spans="2:13" ht="12.75" customHeight="1">
+    <row r="29" spans="2:13" ht="12.2" customHeight="1">
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="23"/>
@@ -45048,7 +45048,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="2:13" ht="13.15" customHeight="1">
+    <row r="30" spans="2:13" ht="12.2" customHeight="1">
       <c r="B30" s="12"/>
       <c r="C30" s="2"/>
       <c r="D30" s="22"/>
@@ -45062,7 +45062,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="2:13" ht="13.15" customHeight="1">
+    <row r="31" spans="2:13" ht="12.2" customHeight="1">
       <c r="B31" s="13"/>
       <c r="C31" s="5"/>
       <c r="D31" s="23"/>
@@ -45076,7 +45076,7 @@
       <c r="L31" s="8"/>
       <c r="M31" s="15"/>
     </row>
-    <row r="32" spans="2:13" ht="13.15" customHeight="1">
+    <row r="32" spans="2:13" ht="12.2" customHeight="1">
       <c r="B32" s="12"/>
       <c r="C32" s="2"/>
       <c r="D32" s="22"/>
@@ -45090,7 +45090,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="16"/>
     </row>
-    <row r="33" spans="2:13" ht="13.15" customHeight="1">
+    <row r="33" spans="2:13" ht="12.2" customHeight="1">
       <c r="B33" s="13"/>
       <c r="C33" s="5"/>
       <c r="D33" s="23"/>
@@ -45104,7 +45104,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="2:13" ht="13.15" customHeight="1">
+    <row r="34" spans="2:13" ht="12.2" customHeight="1">
       <c r="B34" s="12"/>
       <c r="C34" s="2"/>
       <c r="D34" s="22"/>
@@ -45118,7 +45118,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="16"/>
     </row>
-    <row r="35" spans="2:13" ht="13.15" customHeight="1">
+    <row r="35" spans="2:13" ht="12.2" customHeight="1">
       <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="23"/>
@@ -45132,7 +45132,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="2:13" ht="13.15" customHeight="1">
+    <row r="36" spans="2:13" ht="12.2" customHeight="1">
       <c r="B36" s="12"/>
       <c r="C36" s="2"/>
       <c r="D36" s="22"/>
@@ -45146,7 +45146,7 @@
       <c r="L36" s="6"/>
       <c r="M36" s="16"/>
     </row>
-    <row r="37" spans="2:13" ht="13.15" customHeight="1">
+    <row r="37" spans="2:13" ht="12.2" customHeight="1">
       <c r="B37" s="13"/>
       <c r="C37" s="5"/>
       <c r="D37" s="23"/>
@@ -45160,7 +45160,7 @@
       <c r="L37" s="8"/>
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="2:13" ht="13.15" customHeight="1">
+    <row r="38" spans="2:13" ht="12.2" customHeight="1">
       <c r="B38" s="12"/>
       <c r="C38" s="2"/>
       <c r="D38" s="22"/>
@@ -45174,7 +45174,7 @@
       <c r="L38" s="6"/>
       <c r="M38" s="16"/>
     </row>
-    <row r="39" spans="2:13" ht="12.75" customHeight="1">
+    <row r="39" spans="2:13" ht="12.2" customHeight="1">
       <c r="B39" s="13"/>
       <c r="C39" s="5"/>
       <c r="D39" s="23"/>
@@ -45188,7 +45188,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="15"/>
     </row>
-    <row r="40" spans="2:13" ht="13.15" customHeight="1">
+    <row r="40" spans="2:13" ht="12.2" customHeight="1">
       <c r="B40" s="12"/>
       <c r="C40" s="2"/>
       <c r="D40" s="22"/>
@@ -45202,7 +45202,7 @@
       <c r="L40" s="6"/>
       <c r="M40" s="16"/>
     </row>
-    <row r="41" spans="2:13" ht="13.15" customHeight="1">
+    <row r="41" spans="2:13" ht="12.2" customHeight="1">
       <c r="B41" s="13"/>
       <c r="C41" s="5"/>
       <c r="D41" s="23"/>
@@ -45216,7 +45216,7 @@
       <c r="L41" s="8"/>
       <c r="M41" s="15"/>
     </row>
-    <row r="42" spans="2:13" ht="13.15" customHeight="1">
+    <row r="42" spans="2:13" ht="12.2" customHeight="1">
       <c r="B42" s="12"/>
       <c r="C42" s="2"/>
       <c r="D42" s="22"/>
@@ -45230,7 +45230,7 @@
       <c r="L42" s="6"/>
       <c r="M42" s="16"/>
     </row>
-    <row r="43" spans="2:13" ht="13.15" customHeight="1">
+    <row r="43" spans="2:13" ht="12.2" customHeight="1">
       <c r="B43" s="13"/>
       <c r="C43" s="5"/>
       <c r="D43" s="23"/>
@@ -45244,7 +45244,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="15"/>
     </row>
-    <row r="44" spans="2:13" ht="13.15" customHeight="1">
+    <row r="44" spans="2:13" ht="12.2" customHeight="1">
       <c r="B44" s="12"/>
       <c r="C44" s="2"/>
       <c r="D44" s="22"/>
@@ -45258,7 +45258,7 @@
       <c r="L44" s="6"/>
       <c r="M44" s="16"/>
     </row>
-    <row r="45" spans="2:13" ht="13.15" customHeight="1">
+    <row r="45" spans="2:13" ht="12.2" customHeight="1">
       <c r="B45" s="13"/>
       <c r="C45" s="5"/>
       <c r="D45" s="23"/>
@@ -45272,7 +45272,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="2:13" ht="13.15" customHeight="1">
+    <row r="46" spans="2:13" ht="12.2" customHeight="1">
       <c r="B46" s="12"/>
       <c r="C46" s="2"/>
       <c r="D46" s="22"/>
@@ -45286,7 +45286,7 @@
       <c r="L46" s="6"/>
       <c r="M46" s="16"/>
     </row>
-    <row r="47" spans="2:13" ht="13.15" customHeight="1">
+    <row r="47" spans="2:13" ht="12.2" customHeight="1">
       <c r="B47" s="13"/>
       <c r="C47" s="5"/>
       <c r="D47" s="23"/>
@@ -45300,7 +45300,7 @@
       <c r="L47" s="8"/>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="2:13" ht="13.15" customHeight="1">
+    <row r="48" spans="2:13" ht="12.2" customHeight="1">
       <c r="B48" s="12"/>
       <c r="C48" s="2"/>
       <c r="D48" s="22"/>
@@ -45314,7 +45314,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="16"/>
     </row>
-    <row r="49" spans="2:13" ht="12.75" customHeight="1">
+    <row r="49" spans="2:13" ht="12.2" customHeight="1">
       <c r="B49" s="13"/>
       <c r="C49" s="5"/>
       <c r="D49" s="23"/>
@@ -45328,7 +45328,7 @@
       <c r="L49" s="8"/>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="2:13" ht="13.15" customHeight="1">
+    <row r="50" spans="2:13" ht="12.2" customHeight="1">
       <c r="B50" s="12"/>
       <c r="C50" s="2"/>
       <c r="D50" s="22"/>
@@ -45342,7 +45342,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="16"/>
     </row>
-    <row r="51" spans="2:13" ht="12.75" customHeight="1">
+    <row r="51" spans="2:13" ht="12.2" customHeight="1">
       <c r="B51" s="13"/>
       <c r="C51" s="5"/>
       <c r="D51" s="23"/>
@@ -45356,7 +45356,7 @@
       <c r="L51" s="8"/>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="2:13" ht="13.15" customHeight="1">
+    <row r="52" spans="2:13" ht="12.2" customHeight="1">
       <c r="B52" s="12"/>
       <c r="C52" s="2"/>
       <c r="D52" s="22"/>
@@ -45370,7 +45370,7 @@
       <c r="L52" s="6"/>
       <c r="M52" s="16"/>
     </row>
-    <row r="53" spans="2:13" ht="13.15" customHeight="1">
+    <row r="53" spans="2:13" ht="12.2" customHeight="1">
       <c r="B53" s="13"/>
       <c r="C53" s="5"/>
       <c r="D53" s="23"/>
@@ -45384,7 +45384,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="2:13" ht="13.15" customHeight="1">
+    <row r="54" spans="2:13" ht="12.2" customHeight="1">
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="22"/>
@@ -45398,7 +45398,7 @@
       <c r="L54" s="6"/>
       <c r="M54" s="16"/>
     </row>
-    <row r="55" spans="2:13" ht="13.15" customHeight="1">
+    <row r="55" spans="2:13" ht="12.2" customHeight="1">
       <c r="B55" s="13"/>
       <c r="C55" s="5"/>
       <c r="D55" s="23"/>
@@ -45412,7 +45412,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="2:13" ht="13.15" customHeight="1">
+    <row r="56" spans="2:13" ht="12.2" customHeight="1">
       <c r="B56" s="12"/>
       <c r="C56" s="2"/>
       <c r="D56" s="22"/>
@@ -45426,7 +45426,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="16"/>
     </row>
-    <row r="57" spans="2:13" ht="13.15" customHeight="1">
+    <row r="57" spans="2:13" ht="12.2" customHeight="1">
       <c r="B57" s="13"/>
       <c r="C57" s="5"/>
       <c r="D57" s="23"/>
@@ -45440,7 +45440,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="2:13" ht="13.15" customHeight="1">
+    <row r="58" spans="2:13" ht="12.2" customHeight="1">
       <c r="B58" s="12"/>
       <c r="C58" s="2"/>
       <c r="D58" s="22"/>
@@ -45454,7 +45454,7 @@
       <c r="L58" s="6"/>
       <c r="M58" s="16"/>
     </row>
-    <row r="59" spans="2:13" ht="13.15" customHeight="1">
+    <row r="59" spans="2:13" ht="12.2" customHeight="1">
       <c r="B59" s="13"/>
       <c r="C59" s="5"/>
       <c r="D59" s="23"/>
@@ -45468,7 +45468,7 @@
       <c r="L59" s="8"/>
       <c r="M59" s="15"/>
     </row>
-    <row r="60" spans="2:13" ht="13.15" customHeight="1">
+    <row r="60" spans="2:13" ht="12.2" customHeight="1">
       <c r="B60" s="12"/>
       <c r="C60" s="2"/>
       <c r="D60" s="22"/>
@@ -45482,7 +45482,7 @@
       <c r="L60" s="6"/>
       <c r="M60" s="16"/>
     </row>
-    <row r="61" spans="2:13" ht="13.15" customHeight="1">
+    <row r="61" spans="2:13" ht="12.2" customHeight="1">
       <c r="B61" s="13"/>
       <c r="C61" s="5"/>
       <c r="D61" s="23"/>
@@ -45496,7 +45496,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="2:13" ht="13.15" customHeight="1">
+    <row r="62" spans="2:13" ht="12.2" customHeight="1">
       <c r="B62" s="12"/>
       <c r="C62" s="2"/>
       <c r="D62" s="22"/>
@@ -45510,7 +45510,7 @@
       <c r="L62" s="6"/>
       <c r="M62" s="16"/>
     </row>
-    <row r="63" spans="2:13" ht="13.15" customHeight="1">
+    <row r="63" spans="2:13" ht="12.2" customHeight="1">
       <c r="B63" s="13"/>
       <c r="C63" s="5"/>
       <c r="D63" s="23"/>
@@ -45524,7 +45524,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="15"/>
     </row>
-    <row r="64" spans="2:13" ht="13.15" customHeight="1">
+    <row r="64" spans="2:13" ht="12.2" customHeight="1">
       <c r="B64" s="12"/>
       <c r="C64" s="2"/>
       <c r="D64" s="22"/>
@@ -45538,7 +45538,7 @@
       <c r="L64" s="6"/>
       <c r="M64" s="16"/>
     </row>
-    <row r="65" spans="2:13" ht="12.75" customHeight="1">
+    <row r="65" spans="2:13" ht="12.2" customHeight="1">
       <c r="B65" s="13"/>
       <c r="C65" s="5"/>
       <c r="D65" s="23"/>
@@ -45552,7 +45552,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="15"/>
     </row>
-    <row r="66" spans="2:13" ht="13.15" customHeight="1">
+    <row r="66" spans="2:13" ht="12.2" customHeight="1">
       <c r="B66" s="12"/>
       <c r="C66" s="2"/>
       <c r="D66" s="22"/>
@@ -45566,7 +45566,7 @@
       <c r="L66" s="6"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="2:13" ht="13.15" customHeight="1">
+    <row r="67" spans="2:13" ht="12.2" customHeight="1">
       <c r="B67" s="13"/>
       <c r="C67" s="5"/>
       <c r="D67" s="23"/>
@@ -45580,7 +45580,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="15"/>
     </row>
-    <row r="68" spans="2:13" ht="13.15" customHeight="1">
+    <row r="68" spans="2:13" ht="12.2" customHeight="1">
       <c r="B68" s="12"/>
       <c r="C68" s="2"/>
       <c r="D68" s="22"/>
@@ -45594,7 +45594,7 @@
       <c r="L68" s="6"/>
       <c r="M68" s="16"/>
     </row>
-    <row r="69" spans="2:13" ht="13.15" customHeight="1">
+    <row r="69" spans="2:13" ht="12.2" customHeight="1">
       <c r="B69" s="13"/>
       <c r="C69" s="5"/>
       <c r="D69" s="23"/>
@@ -45608,7 +45608,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="15"/>
     </row>
-    <row r="70" spans="2:13" ht="13.15" customHeight="1">
+    <row r="70" spans="2:13" ht="12.2" customHeight="1">
       <c r="B70" s="12"/>
       <c r="C70" s="2"/>
       <c r="D70" s="22"/>
@@ -45622,7 +45622,7 @@
       <c r="L70" s="6"/>
       <c r="M70" s="16"/>
     </row>
-    <row r="71" spans="2:13" ht="13.15" customHeight="1">
+    <row r="71" spans="2:13" ht="12.2" customHeight="1">
       <c r="B71" s="13"/>
       <c r="C71" s="5"/>
       <c r="D71" s="23"/>
@@ -45636,7 +45636,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="15"/>
     </row>
-    <row r="72" spans="2:13" ht="13.15" customHeight="1">
+    <row r="72" spans="2:13" ht="12.2" customHeight="1">
       <c r="B72" s="24"/>
       <c r="C72" s="25"/>
       <c r="D72" s="26"/>
@@ -45650,7 +45650,7 @@
       <c r="L72" s="29"/>
       <c r="M72" s="30"/>
     </row>
-    <row r="73" spans="2:13" ht="13.15" customHeight="1">
+    <row r="73" spans="2:13" ht="12.2" customHeight="1">
       <c r="B73" s="13"/>
       <c r="C73" s="5"/>
       <c r="D73" s="23"/>
@@ -45664,7 +45664,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="15"/>
     </row>
-    <row r="74" spans="2:13" ht="13.15" customHeight="1" thickBot="1">
+    <row r="74" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
       <c r="B74" s="31"/>
       <c r="C74" s="32"/>
       <c r="D74" s="33"/>

</xml_diff>

<commit_message>
Update QMM016 and QMM017
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -44620,9 +44620,7 @@
   </sheetPr>
   <dimension ref="B1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="10" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="I29" sqref="I28:I29"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44634,7 +44632,7 @@
     <col min="6" max="10" width="17.5703125" style="17" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="57.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="1.140625" style="1" customWidth="1"/>
     <col min="15" max="16384" width="10.7109375" style="1"/>
   </cols>

</xml_diff>

<commit_message>
QMM016 Update template + source
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -79,7 +79,7 @@
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$5</definedName>
     <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
     <definedName name="SE単価">[8]明細合計!#REF!</definedName>
@@ -269,7 +269,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,13 +298,6 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
@@ -320,18 +313,12 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -496,51 +483,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="6" tint="0.79998168889431442"/>
       </left>
@@ -584,184 +526,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+  </cellStyleXfs>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="55">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="1"/>
     <cellStyle name="標準 3" xfId="2"/>
@@ -44633,7 +44541,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M75"/>
+  <dimension ref="B1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0"/>
   </sheetViews>
@@ -44644,7 +44552,7 @@
     <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="17.5703125" style="13" customWidth="1"/>
+    <col min="6" max="10" width="17.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
@@ -44654,1044 +44562,78 @@
   <sheetData>
     <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="45" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="39" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B3" s="38"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="44"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B4" s="8"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="12"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B5" s="9"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="11"/>
+    <row r="5" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B6" s="8"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B7" s="9"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="12"/>
-    </row>
-    <row r="9" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B9" s="9"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B10" s="8"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B11" s="9"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B12" s="8"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B13" s="9"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B14" s="8"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B15" s="9"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B16" s="8"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B17" s="9"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B18" s="8"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B19" s="9"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B20" s="8"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B21" s="9"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="11"/>
-    </row>
-    <row r="22" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B22" s="8"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="12"/>
-    </row>
-    <row r="23" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B23" s="9"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="11"/>
-    </row>
-    <row r="24" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B24" s="8"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B25" s="9"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="11"/>
-    </row>
-    <row r="26" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B26" s="8"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B27" s="9"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="11"/>
-    </row>
-    <row r="28" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B28" s="8"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="12"/>
-    </row>
-    <row r="29" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B29" s="9"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="11"/>
-    </row>
-    <row r="30" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B30" s="8"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="12"/>
-    </row>
-    <row r="31" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B31" s="9"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="11"/>
-    </row>
-    <row r="32" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B32" s="8"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="12"/>
-    </row>
-    <row r="33" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B33" s="9"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="11"/>
-    </row>
-    <row r="34" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B34" s="8"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="12"/>
-    </row>
-    <row r="35" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B35" s="9"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="11"/>
-    </row>
-    <row r="36" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B36" s="8"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="12"/>
-    </row>
-    <row r="37" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B37" s="9"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="11"/>
-    </row>
-    <row r="38" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B38" s="8"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="12"/>
-    </row>
-    <row r="39" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B39" s="9"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B40" s="8"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="12"/>
-    </row>
-    <row r="41" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B41" s="9"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="11"/>
-    </row>
-    <row r="42" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B42" s="8"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="12"/>
-    </row>
-    <row r="43" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B43" s="9"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="11"/>
-    </row>
-    <row r="44" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B44" s="8"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="12"/>
-    </row>
-    <row r="45" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B45" s="9"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="11"/>
-    </row>
-    <row r="46" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B46" s="8"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="12"/>
-    </row>
-    <row r="47" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B47" s="9"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="11"/>
-    </row>
-    <row r="48" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B48" s="8"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="12"/>
-    </row>
-    <row r="49" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B49" s="9"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="11"/>
-    </row>
-    <row r="50" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B50" s="8"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="12"/>
-    </row>
-    <row r="51" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B51" s="9"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="11"/>
-    </row>
-    <row r="52" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B52" s="8"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="12"/>
-    </row>
-    <row r="53" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B53" s="9"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="11"/>
-    </row>
-    <row r="54" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B54" s="8"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="12"/>
-    </row>
-    <row r="55" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B55" s="9"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="11"/>
-    </row>
-    <row r="56" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B56" s="8"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="12"/>
-    </row>
-    <row r="57" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B57" s="9"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="11"/>
-    </row>
-    <row r="58" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B58" s="8"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="12"/>
-    </row>
-    <row r="59" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B59" s="9"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="11"/>
-    </row>
-    <row r="60" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B60" s="8"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="12"/>
-    </row>
-    <row r="61" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B61" s="9"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="11"/>
-    </row>
-    <row r="62" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B62" s="8"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="12"/>
-    </row>
-    <row r="63" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B63" s="9"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="11"/>
-    </row>
-    <row r="64" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B64" s="8"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="12"/>
-    </row>
-    <row r="65" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B65" s="9"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="33"/>
-      <c r="M65" s="11"/>
-    </row>
-    <row r="66" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B66" s="8"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="32"/>
-      <c r="M66" s="12"/>
-    </row>
-    <row r="67" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B67" s="9"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="11"/>
-    </row>
-    <row r="68" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B68" s="8"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="32"/>
-      <c r="M68" s="12"/>
-    </row>
-    <row r="69" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B69" s="9"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="33"/>
-      <c r="M69" s="11"/>
-    </row>
-    <row r="70" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B70" s="8"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="32"/>
-      <c r="M70" s="12"/>
-    </row>
-    <row r="71" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B71" s="9"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="33"/>
-      <c r="M71" s="11"/>
-    </row>
-    <row r="72" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B72" s="20"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="23"/>
-      <c r="K72" s="24"/>
-      <c r="L72" s="35"/>
-      <c r="M72" s="25"/>
-    </row>
-    <row r="73" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B73" s="9"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="33"/>
-      <c r="M73" s="11"/>
-    </row>
-    <row r="74" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
-      <c r="B74" s="26"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="29"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="29"/>
-      <c r="J74" s="29"/>
-      <c r="K74" s="30"/>
-      <c r="L74" s="36"/>
-      <c r="M74" s="31"/>
-    </row>
-    <row r="75" spans="2:13" ht="12.75" thickTop="1"/>
+    <row r="6" spans="2:13" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>

</xml_diff>

<commit_message>
Update order and display 016
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -79,7 +79,7 @@
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$74</definedName>
     <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
     <definedName name="SE単価">[8]明細合計!#REF!</definedName>
@@ -313,12 +313,18 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -483,6 +489,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="6" tint="0.79998168889431442"/>
       </left>
@@ -526,51 +577,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -579,12 +585,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,80 +605,98 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -44541,9 +44571,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M6"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44552,7 +44582,7 @@
     <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="17.5703125" style="6" customWidth="1"/>
+    <col min="6" max="10" width="17.5703125" style="10" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
@@ -44562,78 +44592,92 @@
   <sheetData>
     <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="18" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="12" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="17"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
+    <row r="5" spans="2:13" ht="12.2" customHeight="1">
+      <c r="B5" s="7"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="2:13" ht="12.75" thickTop="1"/>
+    <row r="6" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
+      <c r="B6" s="14"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="2:13" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
@@ -44647,7 +44691,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.84424019607843137" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16賃金テーブルの登録 &amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>

</xml_diff>

<commit_message>
Update 016 , 017
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -79,7 +79,7 @@
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$73</definedName>
     <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
     <definedName name="SE単価">[8]明細合計!#REF!</definedName>
@@ -313,18 +313,12 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -489,51 +483,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="6" tint="0.79998168889431442"/>
       </left>
@@ -577,6 +526,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,18 +579,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -605,98 +593,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -730,7 +700,7 @@
       <sheetName val="master"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
@@ -744,7 +714,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6057,17 +6027,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7848,10 +7818,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44224,7 +44194,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44571,7 +44541,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M7"/>
+  <dimension ref="B1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
@@ -44582,7 +44552,7 @@
     <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="17.5703125" style="10" customWidth="1"/>
+    <col min="6" max="10" width="17.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
@@ -44592,92 +44562,78 @@
   <sheetData>
     <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="34" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="28" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B3" s="27"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="33"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="9"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B5" s="7"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="8"/>
+    <row r="5" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
-      <c r="B6" s="14"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="2:13" ht="12.75" thickTop="1"/>
+    <row r="6" spans="2:13" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
@@ -44691,7 +44647,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.84424019607843137" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16賃金テーブルの登録 &amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>

</xml_diff>

<commit_message>
Update order and format file
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -44587,7 +44587,8 @@
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="1.140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.7109375" style="1"/>
+    <col min="15" max="15" width="2" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
@@ -44691,7 +44692,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.84424019607843137" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16賃金テーブルの登録 &amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>

</xml_diff>

<commit_message>
QMM016,QMM017,QMM035 template scale changed
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM016.xlsx
@@ -50,9 +50,9 @@
     <definedName name="ccc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ｃｃｃｃ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="CULC.cal_index_size">[3]!CULC.cal_index_size</definedName>
-    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
@@ -122,33 +122,8 @@
     <definedName name="ユーザー一覧">'[12]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
     <definedName name="ワイドに">[13]!ワイドに</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
-    <definedName name="人日原価">#REF!</definedName>
-    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="住民税115">#REF!</definedName>
-    <definedName name="住民税96">#REF!</definedName>
-    <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="印刷">[14]!印刷</definedName>
     <definedName name="価格表">#REF!</definedName>
-    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
-    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
-    <definedName name="単価">#REF!</definedName>
-    <definedName name="単価種別">#REF!</definedName>
-    <definedName name="印刷">[14]!印刷</definedName>
-    <definedName name="原価">#REF!</definedName>
-    <definedName name="売値">#REF!</definedName>
-    <definedName name="定価">#REF!</definedName>
-    <definedName name="宿泊">#REF!</definedName>
-    <definedName name="宿泊単金">#REF!</definedName>
-    <definedName name="工程別生産性">#REF!</definedName>
-    <definedName name="日帰り">#REF!</definedName>
-    <definedName name="日帰り単金">#REF!</definedName>
-    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
-    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="機種SORT">[15]!機種SORT</definedName>
-    <definedName name="機能別原価">#REF!</definedName>
     <definedName name="画面1">#REF!</definedName>
     <definedName name="画面2">#REF!</definedName>
     <definedName name="画面３">#REF!</definedName>
@@ -156,21 +131,18 @@
     <definedName name="画面5">#REF!</definedName>
     <definedName name="画面6">#REF!</definedName>
     <definedName name="画面7">#REF!</definedName>
-    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
-    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
-    <definedName name="種別">#REF!</definedName>
-    <definedName name="終了">[16]!終了</definedName>
-    <definedName name="見やすく">[13]!見やすく</definedName>
-    <definedName name="見積工数">#REF!</definedName>
     <definedName name="解析">#N/A</definedName>
-    <definedName name="設計書">#N/A</definedName>
-    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
-    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
+    <definedName name="関連表" hidden="1">#REF!</definedName>
+    <definedName name="機種SORT">[15]!機種SORT</definedName>
+    <definedName name="機能別原価">#REF!</definedName>
     <definedName name="銀行の登録48">#REF!</definedName>
     <definedName name="銀行の登録67">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
-    <definedName name="関連表" hidden="1">#REF!</definedName>
-    <definedName name="電車">#REF!</definedName>
+    <definedName name="見やすく">[13]!見やすく</definedName>
+    <definedName name="見積工数">#REF!</definedName>
+    <definedName name="原価">#REF!</definedName>
+    <definedName name="工程別生産性">#REF!</definedName>
     <definedName name="項目名の登録1">#REF!</definedName>
     <definedName name="項目名の登録2">#REF!</definedName>
     <definedName name="項目名の登録3">#REF!</definedName>
@@ -179,7 +151,35 @@
     <definedName name="項目名の登録6">#REF!</definedName>
     <definedName name="項目名の登録7">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
+    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="種別">#REF!</definedName>
+    <definedName name="終了">[16]!終了</definedName>
+    <definedName name="住民税115">#REF!</definedName>
+    <definedName name="住民税96">#REF!</definedName>
+    <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="宿泊">#REF!</definedName>
+    <definedName name="宿泊単金">#REF!</definedName>
+    <definedName name="人日原価">#REF!</definedName>
+    <definedName name="設計書">#N/A</definedName>
+    <definedName name="単価">#REF!</definedName>
+    <definedName name="単価種別">#REF!</definedName>
+    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="定価">#REF!</definedName>
+    <definedName name="電車">#REF!</definedName>
+    <definedName name="日帰り">#REF!</definedName>
+    <definedName name="日帰り単金">#REF!</definedName>
+    <definedName name="売値">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
+    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -269,17 +269,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -44573,26 +44573,26 @@
   </sheetPr>
   <dimension ref="B1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="17.5703125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="59.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="1.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
+    <col min="6" max="10" width="17.625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="59.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.125" style="1" customWidth="1"/>
     <col min="15" max="15" width="2" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.7109375" style="1"/>
+    <col min="16" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1">
+    <row r="1" spans="2:13" ht="12.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:13" ht="12.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
@@ -44622,7 +44622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="12.2" customHeight="1">
+    <row r="3" spans="2:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="27"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -44636,7 +44636,7 @@
       <c r="L3" s="29"/>
       <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="2:13" ht="12.2" customHeight="1">
+    <row r="4" spans="2:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="6"/>
       <c r="C4" s="23"/>
       <c r="D4" s="12"/>
@@ -44650,7 +44650,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="2:13" ht="12.2" customHeight="1">
+    <row r="5" spans="2:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="24"/>
       <c r="D5" s="13"/>
@@ -44664,7 +44664,7 @@
       <c r="L5" s="21"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="2:13" ht="12.2" customHeight="1" thickBot="1">
+    <row r="6" spans="2:13" ht="12.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="14"/>
       <c r="C6" s="25"/>
       <c r="D6" s="15"/>
@@ -44678,7 +44678,7 @@
       <c r="L6" s="22"/>
       <c r="M6" s="19"/>
     </row>
-    <row r="7" spans="2:13" ht="12.75" thickTop="1"/>
+    <row r="7" spans="2:13" ht="12.75" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
@@ -44693,8 +44693,8 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.84424019607843137" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0">
-    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16賃金テーブルの登録 &amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,標準"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,標準"&amp;16賃金テーブルの登録 &amp;R&amp;"ＭＳ ゴシック,標準"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>